<commit_message>
fixed expanse tree levels fixed user admin
</commit_message>
<xml_diff>
--- a/files/kode_matic.xlsx
+++ b/files/kode_matic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pasovni graf prih. in odh." sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="1011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="1062">
   <si>
     <t>Prvi nivo</t>
   </si>
@@ -3127,6 +3127,159 @@
   </si>
   <si>
     <t>Dolgoročni vrednostni papirji, izdani na tujih trgih</t>
+  </si>
+  <si>
+    <t>PREJETA VRAČILA DANIH POSOJIL IN PRODAJA KAPITALSKIH DELEŽEV</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od posameznikov in zasebnikov</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od posameznikov in zasebnikov - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od posameznikov in zasebnikov - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - od javnih skladov</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - od javnih skladov - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - od javnih skladov - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od javnih podjetij in družb, ki so v lasti države ali občin</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od javnih podjetij in družb, ki so v lasti države ali občin – kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od javnih podjetij in družb, ki so v lasti države ali občin – dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - od finančnih institucij</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - od finančnih institucij - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - od finančnih institucij - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od privatnih podjetij</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od privatnih podjetij - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od privatnih podjetij - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejete obresti od danih posojil privatnim podjetjem iz naslova kupnin</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od občin</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od občin – kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od občin – dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - iz tujine</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - iz tujine - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - iz tujine - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - državnemu proračunu</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - državnemu proračunu - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil - državnemu proračunu - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od javnih agencij</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od javnih agencij - kratkoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil od javnih agencij - dolgoročna posojila</t>
+  </si>
+  <si>
+    <t>Prejeta vračila plačanih poroštev</t>
+  </si>
+  <si>
+    <t>Prejeta vračila plačanih poroštev javnim podjetjem in družbam, ki so v lasti države ali občin</t>
+  </si>
+  <si>
+    <t>Prejeta vračila plačanih poroštev privatnim podjetjem</t>
+  </si>
+  <si>
+    <t>Prejeta vračila plačanih poroštev finančnim institucijam</t>
+  </si>
+  <si>
+    <t>Prejeta vračila plačanih poroštev drugim</t>
+  </si>
+  <si>
+    <t>Prodaja kapitalskih deležev</t>
+  </si>
+  <si>
+    <t>Sredstva, pridobljena s prodajo kapitalskih deležev v javnih podjetjih in družbah, ki so v lasti države ali občin</t>
+  </si>
+  <si>
+    <t>Sredstva, pridobljena s prodajo kapitalskih deležev v finančnih institucijah</t>
+  </si>
+  <si>
+    <t>Sredstva, pridobljena s prodajo kapitalskih deležev v privatnih podjetjih</t>
+  </si>
+  <si>
+    <t>Sredstva, pridobljena s prodajo drugih kapitalskih deležev</t>
+  </si>
+  <si>
+    <t>Prejeta vračila namenskega premoženja</t>
+  </si>
+  <si>
+    <t>Sredstva, pridobljena s prodajo drugih kapitalskih deležev doma in v tujini</t>
+  </si>
+  <si>
+    <t>Kupnine iz naslova privatizacije</t>
+  </si>
+  <si>
+    <t>Sredstva kupnin iz naslova privatizacije</t>
+  </si>
+  <si>
+    <t>Prejeta sredstva kupnin iz naslova privatizacije</t>
+  </si>
+  <si>
+    <t>Prejete obresti od vezanih depozitov iz sredstev kupnin</t>
+  </si>
+  <si>
+    <t>Druge prejete obresti iz sredstev kupnin</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih posojil subjektom, vključenim v enotno upravljanje sredstev sistema EZR</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih likvidnostnih posojil subjektom, vključenim v enotno upravljanje sredstev sistema EZR</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih kratkoročnih posojil subjektom, vključenim v enotno upravljanje sredstev sistema EZR</t>
+  </si>
+  <si>
+    <t>Prejeta vračila danih dolgoročnih posojil subjektom, vključenim v enotno upravljanje sredstev sistema EZR</t>
   </si>
 </sst>
 </file>
@@ -3240,7 +3393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3271,6 +3424,9 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3603,8 +3759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B20:K105"/>
   <sheetViews>
-    <sheetView topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27:K29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,7 +4702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B12:G217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="H16" sqref="H16:H19"/>
     </sheetView>
   </sheetViews>
@@ -6436,10 +6592,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B10:I756"/>
+  <dimension ref="B10:I812"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B705" sqref="B705"/>
+    <sheetView tabSelected="1" topLeftCell="F535" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I576" sqref="I576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10804,10 +10960,10 @@
     </row>
     <row r="520" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B520" s="4">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C520" s="4" t="s">
-        <v>368</v>
+        <v>1011</v>
       </c>
       <c r="D520" s="4"/>
       <c r="E520" s="4"/>
@@ -10818,10 +10974,10 @@
     </row>
     <row r="521" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D521" s="8">
-        <v>780</v>
+        <v>750</v>
       </c>
       <c r="E521" s="8" t="s">
-        <v>378</v>
+        <v>1012</v>
       </c>
       <c r="F521" s="8"/>
       <c r="G521" s="8"/>
@@ -10830,1386 +10986,1416 @@
     </row>
     <row r="522" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F522" s="9">
-        <v>7800</v>
+        <v>7500</v>
       </c>
       <c r="G522" s="9" t="s">
-        <v>450</v>
+        <v>1013</v>
       </c>
       <c r="H522" s="9"/>
       <c r="I522" s="9"/>
     </row>
     <row r="523" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H523" s="1">
-        <v>780000</v>
+        <v>750000</v>
       </c>
       <c r="I523" s="1" t="s">
-        <v>450</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="524" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H524" s="1">
-        <v>780001</v>
+        <v>750001</v>
       </c>
       <c r="I524" s="1" t="s">
-        <v>852</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="525" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F525" s="9">
-        <v>7801</v>
+        <v>7501</v>
       </c>
       <c r="G525" s="9" t="s">
-        <v>451</v>
+        <v>1016</v>
       </c>
       <c r="H525" s="9"/>
       <c r="I525" s="9"/>
     </row>
     <row r="526" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H526" s="1">
-        <v>780100</v>
+        <v>750100</v>
       </c>
       <c r="I526" s="1" t="s">
-        <v>451</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="527" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H527" s="1">
-        <v>780101</v>
+        <v>750101</v>
       </c>
       <c r="I527" s="1" t="s">
-        <v>853</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="528" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F528" s="9">
-        <v>7802</v>
+        <v>7502</v>
       </c>
       <c r="G528" s="9" t="s">
-        <v>452</v>
+        <v>1019</v>
       </c>
       <c r="H528" s="9"/>
       <c r="I528" s="9"/>
     </row>
-    <row r="529" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="529" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H529" s="1">
-        <v>780200</v>
+        <v>750200</v>
       </c>
       <c r="I529" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="530" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="530" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H530" s="1">
-        <v>780201</v>
+        <v>750201</v>
       </c>
       <c r="I530" s="1" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="531" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="531" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F531" s="9">
-        <v>7803</v>
+        <v>7503</v>
       </c>
       <c r="G531" s="9" t="s">
-        <v>453</v>
+        <v>1022</v>
       </c>
       <c r="H531" s="9"/>
       <c r="I531" s="9"/>
     </row>
-    <row r="532" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="532" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H532" s="1">
-        <v>780300</v>
+        <v>750300</v>
       </c>
       <c r="I532" s="1" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="533" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="533" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H533" s="1">
-        <v>780301</v>
+        <v>750301</v>
       </c>
       <c r="I533" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="534" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D534" s="8">
-        <v>781</v>
-      </c>
-      <c r="E534" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="F534" s="8"/>
-      <c r="G534" s="8"/>
-      <c r="H534" s="8"/>
-      <c r="I534" s="8"/>
-    </row>
-    <row r="535" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F535" s="9">
-        <v>7810</v>
-      </c>
-      <c r="G535" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="H535" s="9"/>
-      <c r="I535" s="9"/>
-    </row>
-    <row r="536" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="534" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F534" s="9">
+        <v>7504</v>
+      </c>
+      <c r="G534" s="9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H534" s="9"/>
+      <c r="I534" s="9"/>
+    </row>
+    <row r="535" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H535" s="1">
+        <v>750400</v>
+      </c>
+      <c r="I535" s="1" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="536" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H536" s="1">
-        <v>781000</v>
+        <v>750401</v>
       </c>
       <c r="I536" s="1" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="537" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="537" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H537" s="1">
-        <v>781001</v>
+        <v>750402</v>
       </c>
       <c r="I537" s="1" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="538" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H538" s="1">
-        <v>781002</v>
-      </c>
-      <c r="I538" s="1" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="539" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="538" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F538" s="9">
+        <v>7505</v>
+      </c>
+      <c r="G538" s="9" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H538" s="9"/>
+      <c r="I538" s="9"/>
+    </row>
+    <row r="539" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H539" s="1">
-        <v>781003</v>
+        <v>750500</v>
       </c>
       <c r="I539" s="1" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="540" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="540" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H540" s="1">
-        <v>781004</v>
+        <v>750501</v>
       </c>
       <c r="I540" s="1" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="541" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H541" s="1">
-        <v>781005</v>
-      </c>
-      <c r="I541" s="1" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="542" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F542" s="9">
-        <v>7811</v>
-      </c>
-      <c r="G542" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="H542" s="9"/>
-      <c r="I542" s="9"/>
-    </row>
-    <row r="543" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="541" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F541" s="9">
+        <v>7506</v>
+      </c>
+      <c r="G541" s="9" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H541" s="9"/>
+      <c r="I541" s="9"/>
+    </row>
+    <row r="542" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H542" s="1">
+        <v>750600</v>
+      </c>
+      <c r="I542" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="543" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H543" s="1">
-        <v>781100</v>
+        <v>750601</v>
       </c>
       <c r="I543" s="1" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="544" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H544" s="1">
-        <v>781101</v>
-      </c>
-      <c r="I544" s="1" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="545" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="544" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F544" s="9">
+        <v>7507</v>
+      </c>
+      <c r="G544" s="9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H544" s="9"/>
+      <c r="I544" s="9"/>
+    </row>
+    <row r="545" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H545" s="1">
-        <v>781102</v>
+        <v>750700</v>
       </c>
       <c r="I545" s="1" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="546" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="546" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H546" s="1">
-        <v>781103</v>
+        <v>750701</v>
       </c>
       <c r="I546" s="1" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="547" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H547" s="1">
-        <v>781104</v>
-      </c>
-      <c r="I547" s="1" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="548" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="547" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F547" s="9">
+        <v>7508</v>
+      </c>
+      <c r="G547" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="H547" s="9"/>
+      <c r="I547" s="9"/>
+    </row>
+    <row r="548" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H548" s="1">
-        <v>781105</v>
+        <v>750800</v>
       </c>
       <c r="I548" s="1" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="549" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F549" s="9">
-        <v>7812</v>
-      </c>
-      <c r="G549" s="9" t="s">
-        <v>456</v>
-      </c>
-      <c r="H549" s="9"/>
-      <c r="I549" s="9"/>
-    </row>
-    <row r="550" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H550" s="1">
-        <v>781200</v>
-      </c>
-      <c r="I550" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="551" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="549" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H549" s="1">
+        <v>750801</v>
+      </c>
+      <c r="I549" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="550" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F550" s="9">
+        <v>7509</v>
+      </c>
+      <c r="G550" s="9" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H550" s="9"/>
+      <c r="I550" s="9"/>
+    </row>
+    <row r="551" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H551" s="1">
-        <v>781201</v>
+        <v>750900</v>
       </c>
       <c r="I551" s="1" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="552" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="552" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H552" s="1">
-        <v>781202</v>
+        <v>750901</v>
       </c>
       <c r="I552" s="1" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="553" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="553" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H553" s="1">
-        <v>781203</v>
+        <v>750902</v>
       </c>
       <c r="I553" s="1" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="554" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="554" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H554" s="1">
-        <v>781204</v>
+        <v>750999</v>
       </c>
       <c r="I554" s="1" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="555" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H555" s="1">
-        <v>781205</v>
-      </c>
-      <c r="I555" s="1" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="556" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H556" s="1">
-        <v>781206</v>
-      </c>
-      <c r="I556" s="1" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="557" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="555" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D555" s="8">
+        <v>751</v>
+      </c>
+      <c r="E555" s="8" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F555" s="8"/>
+      <c r="G555" s="8"/>
+      <c r="H555" s="8"/>
+      <c r="I555" s="8"/>
+    </row>
+    <row r="556" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F556" s="9">
+        <v>7510</v>
+      </c>
+      <c r="G556" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H556" s="9"/>
+      <c r="I556" s="9"/>
+    </row>
+    <row r="557" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H557" s="1">
-        <v>781207</v>
+        <v>751000</v>
       </c>
       <c r="I557" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="558" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H558" s="1">
-        <v>781208</v>
-      </c>
-      <c r="I558" s="1" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="559" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="558" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F558" s="9">
+        <v>7511</v>
+      </c>
+      <c r="G558" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H558" s="9"/>
+      <c r="I558" s="9"/>
+    </row>
+    <row r="559" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H559" s="1">
-        <v>781209</v>
+        <v>751100</v>
       </c>
       <c r="I559" s="1" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="560" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H560" s="1">
-        <v>781210</v>
-      </c>
-      <c r="I560" s="1" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="561" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="560" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F560" s="9">
+        <v>7512</v>
+      </c>
+      <c r="G560" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H560" s="9"/>
+      <c r="I560" s="9"/>
+    </row>
+    <row r="561" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H561" s="1">
-        <v>781211</v>
+        <v>751200</v>
       </c>
       <c r="I561" s="1" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="562" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="562" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F562" s="9">
-        <v>7813</v>
+        <v>7513</v>
       </c>
       <c r="G562" s="9" t="s">
-        <v>457</v>
+        <v>1050</v>
       </c>
       <c r="H562" s="9"/>
       <c r="I562" s="9"/>
     </row>
-    <row r="563" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="563" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H563" s="1">
-        <v>781300</v>
+        <v>751300</v>
       </c>
       <c r="I563" s="1" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="564" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H564" s="1">
-        <v>781301</v>
-      </c>
-      <c r="I564" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="565" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="564" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F564" s="9">
+        <v>7514</v>
+      </c>
+      <c r="G564" s="9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H564" s="9"/>
+      <c r="I564" s="9"/>
+    </row>
+    <row r="565" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H565" s="1">
-        <v>781302</v>
+        <v>751400</v>
       </c>
       <c r="I565" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="566" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H566" s="1">
-        <v>781303</v>
-      </c>
-      <c r="I566" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="567" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H567" s="1">
-        <v>781304</v>
-      </c>
-      <c r="I567" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="568" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="566" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D566" s="8">
+        <v>752</v>
+      </c>
+      <c r="E566" s="8" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F566" s="8"/>
+      <c r="G566" s="8"/>
+      <c r="H566" s="8"/>
+      <c r="I566" s="8"/>
+    </row>
+    <row r="567" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F567" s="9">
+        <v>7520</v>
+      </c>
+      <c r="G567" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="H567" s="9"/>
+      <c r="I567" s="9"/>
+    </row>
+    <row r="568" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H568" s="1">
-        <v>781305</v>
+        <v>752000</v>
       </c>
       <c r="I568" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="569" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="569" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H569" s="1">
-        <v>781306</v>
+        <v>752001</v>
       </c>
       <c r="I569" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="570" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="570" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H570" s="1">
-        <v>781307</v>
+        <v>752002</v>
       </c>
       <c r="I570" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="571" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H571" s="1">
-        <v>781308</v>
-      </c>
-      <c r="I571" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="572" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H572" s="1">
-        <v>781309</v>
-      </c>
-      <c r="I572" s="1" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="573" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="571" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D571" s="8">
+        <v>753</v>
+      </c>
+      <c r="E571" s="8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F571" s="8"/>
+      <c r="G571" s="8"/>
+      <c r="H571" s="8"/>
+      <c r="I571" s="8"/>
+    </row>
+    <row r="572" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F572" s="9">
+        <v>7530</v>
+      </c>
+      <c r="G572" s="9" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H572" s="9"/>
+      <c r="I572" s="9"/>
+    </row>
+    <row r="573" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H573" s="1">
-        <v>781310</v>
+        <v>753000</v>
       </c>
       <c r="I573" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="574" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="574" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H574" s="1">
-        <v>781311</v>
+        <v>753001</v>
       </c>
       <c r="I574" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="575" spans="6:9" x14ac:dyDescent="0.25">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="575" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H575" s="1">
-        <v>781312</v>
-      </c>
-      <c r="I575" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="576" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H576" s="1">
-        <v>781399</v>
-      </c>
-      <c r="I576" s="1" t="s">
-        <v>457</v>
-      </c>
+        <v>753002</v>
+      </c>
+      <c r="I575" s="21" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="576" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B576" s="4">
+        <v>78</v>
+      </c>
+      <c r="C576" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D576" s="4"/>
+      <c r="E576" s="4"/>
+      <c r="F576" s="4"/>
+      <c r="G576" s="4"/>
+      <c r="H576" s="4"/>
+      <c r="I576" s="4"/>
     </row>
     <row r="577" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F577" s="9">
-        <v>7814</v>
-      </c>
-      <c r="G577" s="9" t="s">
-        <v>458</v>
-      </c>
-      <c r="H577" s="9"/>
-      <c r="I577" s="9"/>
+      <c r="D577" s="8">
+        <v>780</v>
+      </c>
+      <c r="E577" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="F577" s="8"/>
+      <c r="G577" s="8"/>
+      <c r="H577" s="8"/>
+      <c r="I577" s="8"/>
     </row>
     <row r="578" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H578" s="1">
-        <v>781400</v>
-      </c>
-      <c r="I578" s="1" t="s">
-        <v>882</v>
-      </c>
+      <c r="F578" s="9">
+        <v>7800</v>
+      </c>
+      <c r="G578" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="H578" s="9"/>
+      <c r="I578" s="9"/>
     </row>
     <row r="579" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H579" s="1">
-        <v>781401</v>
+        <v>780000</v>
       </c>
       <c r="I579" s="1" t="s">
-        <v>359</v>
+        <v>450</v>
       </c>
     </row>
     <row r="580" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H580" s="1">
-        <v>781402</v>
+        <v>780001</v>
       </c>
       <c r="I580" s="1" t="s">
-        <v>883</v>
+        <v>852</v>
       </c>
     </row>
     <row r="581" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H581" s="1">
-        <v>781403</v>
-      </c>
-      <c r="I581" s="1" t="s">
-        <v>884</v>
-      </c>
+      <c r="F581" s="9">
+        <v>7801</v>
+      </c>
+      <c r="G581" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="H581" s="9"/>
+      <c r="I581" s="9"/>
     </row>
     <row r="582" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H582" s="1">
-        <v>781404</v>
+        <v>780100</v>
       </c>
       <c r="I582" s="1" t="s">
-        <v>360</v>
+        <v>451</v>
       </c>
     </row>
     <row r="583" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D583" s="8">
-        <v>782</v>
-      </c>
-      <c r="E583" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F583" s="8"/>
-      <c r="G583" s="8"/>
-      <c r="H583" s="8"/>
-      <c r="I583" s="8"/>
+      <c r="H583" s="1">
+        <v>780101</v>
+      </c>
+      <c r="I583" s="1" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="584" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F584" s="9">
-        <v>7820</v>
+        <v>7802</v>
       </c>
       <c r="G584" s="9" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="H584" s="9"/>
       <c r="I584" s="9"/>
     </row>
     <row r="585" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H585" s="1">
-        <v>782000</v>
+        <v>780200</v>
       </c>
       <c r="I585" s="1" t="s">
-        <v>885</v>
+        <v>452</v>
       </c>
     </row>
     <row r="586" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H586" s="1">
-        <v>782001</v>
+        <v>780201</v>
       </c>
       <c r="I586" s="1" t="s">
-        <v>886</v>
+        <v>854</v>
       </c>
     </row>
     <row r="587" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H587" s="1">
-        <v>782002</v>
-      </c>
-      <c r="I587" s="1" t="s">
-        <v>887</v>
-      </c>
+      <c r="F587" s="9">
+        <v>7803</v>
+      </c>
+      <c r="G587" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="H587" s="9"/>
+      <c r="I587" s="9"/>
     </row>
     <row r="588" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H588" s="1">
-        <v>782003</v>
+        <v>780300</v>
       </c>
       <c r="I588" s="1" t="s">
-        <v>888</v>
+        <v>855</v>
       </c>
     </row>
     <row r="589" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F589" s="9">
-        <v>7821</v>
-      </c>
-      <c r="G589" s="9" t="s">
-        <v>460</v>
-      </c>
-      <c r="H589" s="9"/>
-      <c r="I589" s="9"/>
+      <c r="H589" s="1">
+        <v>780301</v>
+      </c>
+      <c r="I589" s="1" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="590" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H590" s="1">
-        <v>782100</v>
-      </c>
-      <c r="I590" s="1" t="s">
-        <v>889</v>
-      </c>
+      <c r="D590" s="8">
+        <v>781</v>
+      </c>
+      <c r="E590" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="F590" s="8"/>
+      <c r="G590" s="8"/>
+      <c r="H590" s="8"/>
+      <c r="I590" s="8"/>
     </row>
     <row r="591" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H591" s="1">
-        <v>782101</v>
-      </c>
-      <c r="I591" s="1" t="s">
-        <v>890</v>
-      </c>
+      <c r="F591" s="9">
+        <v>7810</v>
+      </c>
+      <c r="G591" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="H591" s="9"/>
+      <c r="I591" s="9"/>
     </row>
     <row r="592" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H592" s="1">
-        <v>782102</v>
+        <v>781000</v>
       </c>
       <c r="I592" s="1" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="593" spans="8:9" x14ac:dyDescent="0.25">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="593" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H593" s="1">
-        <v>782103</v>
+        <v>781001</v>
       </c>
       <c r="I593" s="1" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="594" spans="8:9" x14ac:dyDescent="0.25">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="594" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H594" s="1">
-        <v>782104</v>
+        <v>781002</v>
       </c>
       <c r="I594" s="1" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="595" spans="8:9" x14ac:dyDescent="0.25">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="595" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H595" s="1">
-        <v>782105</v>
+        <v>781003</v>
       </c>
       <c r="I595" s="1" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="596" spans="8:9" x14ac:dyDescent="0.25">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="596" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H596" s="1">
-        <v>782106</v>
+        <v>781004</v>
       </c>
       <c r="I596" s="1" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="597" spans="8:9" x14ac:dyDescent="0.25">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="597" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H597" s="1">
-        <v>782107</v>
+        <v>781005</v>
       </c>
       <c r="I597" s="1" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="598" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H598" s="1">
-        <v>782108</v>
-      </c>
-      <c r="I598" s="1" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="599" spans="8:9" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="598" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F598" s="9">
+        <v>7811</v>
+      </c>
+      <c r="G598" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="H598" s="9"/>
+      <c r="I598" s="9"/>
+    </row>
+    <row r="599" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H599" s="1">
-        <v>782109</v>
+        <v>781100</v>
       </c>
       <c r="I599" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="600" spans="8:9" x14ac:dyDescent="0.25">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="600" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H600" s="1">
-        <v>782110</v>
+        <v>781101</v>
       </c>
       <c r="I600" s="1" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="601" spans="8:9" x14ac:dyDescent="0.25">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="601" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H601" s="1">
-        <v>782111</v>
+        <v>781102</v>
       </c>
       <c r="I601" s="1" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="602" spans="8:9" x14ac:dyDescent="0.25">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="602" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H602" s="1">
-        <v>782112</v>
+        <v>781103</v>
       </c>
       <c r="I602" s="1" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="603" spans="8:9" x14ac:dyDescent="0.25">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="603" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H603" s="1">
-        <v>782113</v>
+        <v>781104</v>
       </c>
       <c r="I603" s="1" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="604" spans="8:9" x14ac:dyDescent="0.25">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="604" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H604" s="1">
-        <v>782114</v>
+        <v>781105</v>
       </c>
       <c r="I604" s="1" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="605" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H605" s="1">
-        <v>782115</v>
-      </c>
-      <c r="I605" s="1" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="606" spans="8:9" x14ac:dyDescent="0.25">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="605" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F605" s="9">
+        <v>7812</v>
+      </c>
+      <c r="G605" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="H605" s="9"/>
+      <c r="I605" s="9"/>
+    </row>
+    <row r="606" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H606" s="1">
-        <v>782116</v>
+        <v>781200</v>
       </c>
       <c r="I606" s="1" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="607" spans="8:9" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="607" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H607" s="1">
-        <v>782117</v>
+        <v>781201</v>
       </c>
       <c r="I607" s="1" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="608" spans="8:9" x14ac:dyDescent="0.25">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="608" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H608" s="1">
-        <v>782118</v>
+        <v>781202</v>
       </c>
       <c r="I608" s="1" t="s">
-        <v>906</v>
+        <v>870</v>
       </c>
     </row>
     <row r="609" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H609" s="1">
-        <v>782119</v>
+        <v>781203</v>
       </c>
       <c r="I609" s="1" t="s">
-        <v>907</v>
+        <v>871</v>
       </c>
     </row>
     <row r="610" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H610" s="1">
-        <v>782120</v>
+        <v>781204</v>
       </c>
       <c r="I610" s="1" t="s">
-        <v>908</v>
+        <v>872</v>
       </c>
     </row>
     <row r="611" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H611" s="1">
-        <v>782121</v>
+        <v>781205</v>
       </c>
       <c r="I611" s="1" t="s">
-        <v>909</v>
+        <v>873</v>
       </c>
     </row>
     <row r="612" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F612" s="9">
-        <v>7822</v>
-      </c>
-      <c r="G612" s="9" t="s">
-        <v>461</v>
-      </c>
-      <c r="H612" s="9"/>
-      <c r="I612" s="9"/>
+      <c r="H612" s="1">
+        <v>781206</v>
+      </c>
+      <c r="I612" s="1" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="613" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H613" s="1">
-        <v>782200</v>
+        <v>781207</v>
       </c>
       <c r="I613" s="1" t="s">
-        <v>910</v>
+        <v>875</v>
       </c>
     </row>
     <row r="614" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H614" s="1">
-        <v>782201</v>
+        <v>781208</v>
       </c>
       <c r="I614" s="1" t="s">
-        <v>911</v>
+        <v>876</v>
       </c>
     </row>
     <row r="615" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H615" s="1">
-        <v>782202</v>
+        <v>781209</v>
       </c>
       <c r="I615" s="1" t="s">
-        <v>912</v>
+        <v>877</v>
       </c>
     </row>
     <row r="616" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H616" s="1">
-        <v>782203</v>
+        <v>781210</v>
       </c>
       <c r="I616" s="1" t="s">
-        <v>913</v>
+        <v>878</v>
       </c>
     </row>
     <row r="617" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H617" s="1">
-        <v>782204</v>
+        <v>781211</v>
       </c>
       <c r="I617" s="1" t="s">
-        <v>914</v>
+        <v>879</v>
       </c>
     </row>
     <row r="618" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H618" s="1">
-        <v>782205</v>
-      </c>
-      <c r="I618" s="1" t="s">
-        <v>915</v>
-      </c>
+      <c r="F618" s="9">
+        <v>7813</v>
+      </c>
+      <c r="G618" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="H618" s="9"/>
+      <c r="I618" s="9"/>
     </row>
     <row r="619" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H619" s="1">
-        <v>782206</v>
+        <v>781300</v>
       </c>
       <c r="I619" s="1" t="s">
-        <v>916</v>
+        <v>880</v>
       </c>
     </row>
     <row r="620" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H620" s="1">
-        <v>782207</v>
+        <v>781301</v>
       </c>
       <c r="I620" s="1" t="s">
-        <v>917</v>
+        <v>348</v>
       </c>
     </row>
     <row r="621" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F621" s="9">
-        <v>7823</v>
-      </c>
-      <c r="G621" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="H621" s="9"/>
-      <c r="I621" s="9"/>
+      <c r="H621" s="1">
+        <v>781302</v>
+      </c>
+      <c r="I621" s="1" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="622" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H622" s="1">
-        <v>782300</v>
+        <v>781303</v>
       </c>
       <c r="I622" s="1" t="s">
-        <v>918</v>
+        <v>350</v>
       </c>
     </row>
     <row r="623" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H623" s="1">
-        <v>782301</v>
+        <v>781304</v>
       </c>
       <c r="I623" s="1" t="s">
-        <v>919</v>
+        <v>351</v>
       </c>
     </row>
     <row r="624" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F624" s="9">
-        <v>7824</v>
-      </c>
-      <c r="G624" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="H624" s="9"/>
-      <c r="I624" s="9"/>
+      <c r="H624" s="1">
+        <v>781305</v>
+      </c>
+      <c r="I624" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="625" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H625" s="1">
-        <v>782400</v>
+        <v>781306</v>
       </c>
       <c r="I625" s="1" t="s">
-        <v>920</v>
+        <v>353</v>
       </c>
     </row>
     <row r="626" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H626" s="1">
-        <v>782401</v>
+        <v>781307</v>
       </c>
       <c r="I626" s="1" t="s">
-        <v>921</v>
+        <v>354</v>
       </c>
     </row>
     <row r="627" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F627" s="9">
-        <v>7825</v>
-      </c>
-      <c r="G627" s="9" t="s">
-        <v>464</v>
-      </c>
-      <c r="H627" s="9"/>
-      <c r="I627" s="9"/>
+      <c r="H627" s="1">
+        <v>781308</v>
+      </c>
+      <c r="I627" s="1" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="628" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H628" s="1">
-        <v>782500</v>
+        <v>781309</v>
       </c>
       <c r="I628" s="1" t="s">
-        <v>922</v>
+        <v>881</v>
       </c>
     </row>
     <row r="629" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H629" s="1">
-        <v>782501</v>
+        <v>781310</v>
       </c>
       <c r="I629" s="1" t="s">
-        <v>923</v>
+        <v>356</v>
       </c>
     </row>
     <row r="630" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D630" s="8">
-        <v>783</v>
-      </c>
-      <c r="E630" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="F630" s="8"/>
-      <c r="G630" s="8"/>
-      <c r="H630" s="8"/>
-      <c r="I630" s="8"/>
+      <c r="H630" s="1">
+        <v>781311</v>
+      </c>
+      <c r="I630" s="1" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="631" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F631" s="9">
-        <v>7830</v>
-      </c>
-      <c r="G631" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="H631" s="9"/>
-      <c r="I631" s="9"/>
+      <c r="H631" s="1">
+        <v>781312</v>
+      </c>
+      <c r="I631" s="1" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="632" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H632" s="1">
-        <v>783000</v>
+        <v>781399</v>
       </c>
       <c r="I632" s="1" t="s">
-        <v>924</v>
+        <v>457</v>
       </c>
     </row>
     <row r="633" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H633" s="1">
-        <v>783001</v>
-      </c>
-      <c r="I633" s="1" t="s">
-        <v>925</v>
-      </c>
+      <c r="F633" s="9">
+        <v>7814</v>
+      </c>
+      <c r="G633" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="H633" s="9"/>
+      <c r="I633" s="9"/>
     </row>
     <row r="634" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H634" s="1">
-        <v>783002</v>
+        <v>781400</v>
       </c>
       <c r="I634" s="1" t="s">
-        <v>926</v>
+        <v>882</v>
       </c>
     </row>
     <row r="635" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H635" s="1">
-        <v>783003</v>
+        <v>781401</v>
       </c>
       <c r="I635" s="1" t="s">
-        <v>927</v>
+        <v>359</v>
       </c>
     </row>
     <row r="636" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H636" s="1">
-        <v>783004</v>
+        <v>781402</v>
       </c>
       <c r="I636" s="1" t="s">
-        <v>928</v>
+        <v>883</v>
       </c>
     </row>
     <row r="637" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H637" s="1">
-        <v>783005</v>
+        <v>781403</v>
       </c>
       <c r="I637" s="1" t="s">
-        <v>362</v>
+        <v>884</v>
       </c>
     </row>
     <row r="638" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H638" s="1">
-        <v>783006</v>
+        <v>781404</v>
       </c>
       <c r="I638" s="1" t="s">
-        <v>929</v>
+        <v>360</v>
       </c>
     </row>
     <row r="639" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H639" s="1">
-        <v>783007</v>
-      </c>
-      <c r="I639" s="1" t="s">
-        <v>930</v>
-      </c>
+      <c r="D639" s="8">
+        <v>782</v>
+      </c>
+      <c r="E639" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F639" s="8"/>
+      <c r="G639" s="8"/>
+      <c r="H639" s="8"/>
+      <c r="I639" s="8"/>
     </row>
     <row r="640" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D640" s="8">
-        <v>784</v>
-      </c>
-      <c r="E640" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="F640" s="8"/>
-      <c r="G640" s="8"/>
-      <c r="H640" s="8"/>
-      <c r="I640" s="8"/>
+      <c r="F640" s="9">
+        <v>7820</v>
+      </c>
+      <c r="G640" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="H640" s="9"/>
+      <c r="I640" s="9"/>
     </row>
     <row r="641" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F641" s="9">
-        <v>7840</v>
-      </c>
-      <c r="G641" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="H641" s="9"/>
-      <c r="I641" s="9"/>
+      <c r="H641" s="1">
+        <v>782000</v>
+      </c>
+      <c r="I641" s="1" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="642" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H642" s="1">
-        <v>784000</v>
+        <v>782001</v>
       </c>
       <c r="I642" s="1" t="s">
-        <v>466</v>
+        <v>886</v>
       </c>
     </row>
     <row r="643" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H643" s="1">
-        <v>784001</v>
+        <v>782002</v>
       </c>
       <c r="I643" s="1" t="s">
-        <v>931</v>
+        <v>887</v>
       </c>
     </row>
     <row r="644" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F644" s="9">
-        <v>7841</v>
-      </c>
-      <c r="G644" s="9" t="s">
-        <v>467</v>
-      </c>
-      <c r="H644" s="9"/>
-      <c r="I644" s="9"/>
+      <c r="H644" s="1">
+        <v>782003</v>
+      </c>
+      <c r="I644" s="1" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="645" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H645" s="1">
-        <v>784100</v>
-      </c>
-      <c r="I645" s="1" t="s">
-        <v>467</v>
-      </c>
+      <c r="F645" s="9">
+        <v>7821</v>
+      </c>
+      <c r="G645" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="H645" s="9"/>
+      <c r="I645" s="9"/>
     </row>
     <row r="646" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H646" s="1">
-        <v>784101</v>
+        <v>782100</v>
       </c>
       <c r="I646" s="1" t="s">
-        <v>932</v>
+        <v>889</v>
       </c>
     </row>
     <row r="647" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F647" s="9">
-        <v>7842</v>
-      </c>
-      <c r="G647" s="9" t="s">
-        <v>468</v>
-      </c>
-      <c r="H647" s="9"/>
-      <c r="I647" s="9"/>
+      <c r="H647" s="1">
+        <v>782101</v>
+      </c>
+      <c r="I647" s="1" t="s">
+        <v>890</v>
+      </c>
     </row>
     <row r="648" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H648" s="1">
-        <v>784200</v>
+        <v>782102</v>
       </c>
       <c r="I648" s="1" t="s">
-        <v>933</v>
+        <v>891</v>
       </c>
     </row>
     <row r="649" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H649" s="1">
-        <v>784201</v>
+        <v>782103</v>
       </c>
       <c r="I649" s="1" t="s">
-        <v>934</v>
+        <v>892</v>
       </c>
     </row>
     <row r="650" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H650" s="1">
-        <v>784202</v>
+        <v>782104</v>
       </c>
       <c r="I650" s="1" t="s">
-        <v>935</v>
+        <v>893</v>
       </c>
     </row>
     <row r="651" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H651" s="1">
-        <v>784203</v>
+        <v>782105</v>
       </c>
       <c r="I651" s="1" t="s">
-        <v>936</v>
+        <v>894</v>
       </c>
     </row>
     <row r="652" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H652" s="1">
-        <v>784204</v>
+        <v>782106</v>
       </c>
       <c r="I652" s="1" t="s">
-        <v>937</v>
+        <v>895</v>
       </c>
     </row>
     <row r="653" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H653" s="1">
-        <v>784205</v>
+        <v>782107</v>
       </c>
       <c r="I653" s="1" t="s">
-        <v>938</v>
+        <v>896</v>
       </c>
     </row>
     <row r="654" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H654" s="1">
-        <v>784206</v>
+        <v>782108</v>
       </c>
       <c r="I654" s="1" t="s">
-        <v>939</v>
+        <v>897</v>
       </c>
     </row>
     <row r="655" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H655" s="1">
-        <v>784207</v>
+        <v>782109</v>
       </c>
       <c r="I655" s="1" t="s">
-        <v>940</v>
+        <v>361</v>
       </c>
     </row>
     <row r="656" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F656" s="9">
-        <v>7843</v>
-      </c>
-      <c r="G656" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="H656" s="9"/>
-      <c r="I656" s="9"/>
-    </row>
-    <row r="657" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H656" s="1">
+        <v>782110</v>
+      </c>
+      <c r="I656" s="1" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="657" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H657" s="1">
-        <v>784300</v>
+        <v>782111</v>
       </c>
       <c r="I657" s="1" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="658" spans="8:9" x14ac:dyDescent="0.25">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="658" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H658" s="1">
-        <v>784301</v>
+        <v>782112</v>
       </c>
       <c r="I658" s="1" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="659" spans="8:9" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="659" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H659" s="1">
-        <v>784302</v>
+        <v>782113</v>
       </c>
       <c r="I659" s="1" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="660" spans="8:9" x14ac:dyDescent="0.25">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="660" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H660" s="1">
-        <v>784303</v>
+        <v>782114</v>
       </c>
       <c r="I660" s="1" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="661" spans="8:9" x14ac:dyDescent="0.25">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="661" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H661" s="1">
-        <v>784304</v>
+        <v>782115</v>
       </c>
       <c r="I661" s="1" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="662" spans="8:9" x14ac:dyDescent="0.25">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="662" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H662" s="1">
-        <v>784305</v>
+        <v>782116</v>
       </c>
       <c r="I662" s="1" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="663" spans="8:9" x14ac:dyDescent="0.25">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="663" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H663" s="1">
-        <v>784306</v>
+        <v>782117</v>
       </c>
       <c r="I663" s="1" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="664" spans="8:9" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="664" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H664" s="1">
-        <v>784307</v>
+        <v>782118</v>
       </c>
       <c r="I664" s="1" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="665" spans="8:9" x14ac:dyDescent="0.25">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="665" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H665" s="1">
-        <v>784308</v>
+        <v>782119</v>
       </c>
       <c r="I665" s="1" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="666" spans="8:9" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="666" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H666" s="1">
-        <v>784309</v>
+        <v>782120</v>
       </c>
       <c r="I666" s="1" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="667" spans="8:9" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="667" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H667" s="1">
-        <v>784310</v>
+        <v>782121</v>
       </c>
       <c r="I667" s="1" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="668" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H668" s="1">
-        <v>784311</v>
-      </c>
-      <c r="I668" s="1" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="669" spans="8:9" x14ac:dyDescent="0.25">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="668" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F668" s="9">
+        <v>7822</v>
+      </c>
+      <c r="G668" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="H668" s="9"/>
+      <c r="I668" s="9"/>
+    </row>
+    <row r="669" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H669" s="1">
-        <v>784312</v>
+        <v>782200</v>
       </c>
       <c r="I669" s="1" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="670" spans="8:9" x14ac:dyDescent="0.25">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="670" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H670" s="1">
-        <v>784313</v>
+        <v>782201</v>
       </c>
       <c r="I670" s="1" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="671" spans="8:9" x14ac:dyDescent="0.25">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="671" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H671" s="1">
-        <v>784314</v>
+        <v>782202</v>
       </c>
       <c r="I671" s="1" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="672" spans="8:9" x14ac:dyDescent="0.25">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="672" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H672" s="1">
-        <v>784315</v>
+        <v>782203</v>
       </c>
       <c r="I672" s="1" t="s">
-        <v>956</v>
+        <v>913</v>
       </c>
     </row>
     <row r="673" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H673" s="1">
-        <v>784316</v>
+        <v>782204</v>
       </c>
       <c r="I673" s="1" t="s">
-        <v>957</v>
+        <v>914</v>
       </c>
     </row>
     <row r="674" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H674" s="1">
-        <v>784317</v>
+        <v>782205</v>
       </c>
       <c r="I674" s="1" t="s">
-        <v>958</v>
+        <v>915</v>
       </c>
     </row>
     <row r="675" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H675" s="1">
-        <v>784318</v>
+        <v>782206</v>
       </c>
       <c r="I675" s="1" t="s">
-        <v>959</v>
+        <v>916</v>
       </c>
     </row>
     <row r="676" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H676" s="1">
-        <v>784319</v>
+        <v>782207</v>
       </c>
       <c r="I676" s="1" t="s">
-        <v>960</v>
+        <v>917</v>
       </c>
     </row>
     <row r="677" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H677" s="1">
-        <v>784320</v>
-      </c>
-      <c r="I677" s="1" t="s">
-        <v>961</v>
-      </c>
+      <c r="F677" s="9">
+        <v>7823</v>
+      </c>
+      <c r="G677" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="H677" s="9"/>
+      <c r="I677" s="9"/>
     </row>
     <row r="678" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H678" s="1">
-        <v>784321</v>
+        <v>782300</v>
       </c>
       <c r="I678" s="1" t="s">
-        <v>962</v>
+        <v>918</v>
       </c>
     </row>
     <row r="679" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D679" s="8">
-        <v>785</v>
-      </c>
-      <c r="E679" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="F679" s="8"/>
-      <c r="G679" s="8"/>
-      <c r="H679" s="8"/>
-      <c r="I679" s="8"/>
+      <c r="H679" s="1">
+        <v>782301</v>
+      </c>
+      <c r="I679" s="1" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="680" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F680" s="9">
-        <v>7850</v>
+        <v>7824</v>
       </c>
       <c r="G680" s="9" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="H680" s="9"/>
       <c r="I680" s="9"/>
     </row>
     <row r="681" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H681" s="1">
-        <v>785000</v>
+        <v>782400</v>
       </c>
       <c r="I681" s="1" t="s">
-        <v>470</v>
+        <v>920</v>
       </c>
     </row>
     <row r="682" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H682" s="1">
-        <v>785001</v>
+        <v>782401</v>
       </c>
       <c r="I682" s="1" t="s">
-        <v>963</v>
+        <v>921</v>
       </c>
     </row>
     <row r="683" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F683" s="9">
-        <v>7851</v>
+        <v>7825</v>
       </c>
       <c r="G683" s="9" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="H683" s="9"/>
       <c r="I683" s="9"/>
     </row>
     <row r="684" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H684" s="1">
-        <v>785100</v>
+        <v>782500</v>
       </c>
       <c r="I684" s="1" t="s">
-        <v>471</v>
+        <v>922</v>
       </c>
     </row>
     <row r="685" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H685" s="1">
-        <v>785101</v>
+        <v>782501</v>
       </c>
       <c r="I685" s="1" t="s">
-        <v>964</v>
+        <v>923</v>
       </c>
     </row>
     <row r="686" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D686" s="8">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E686" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F686" s="8"/>
       <c r="G686" s="8"/>
@@ -12218,627 +12404,1101 @@
     </row>
     <row r="687" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F687" s="9">
-        <v>7860</v>
+        <v>7830</v>
       </c>
       <c r="G687" s="9" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="H687" s="9"/>
       <c r="I687" s="9"/>
     </row>
     <row r="688" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H688" s="1">
-        <v>786000</v>
+        <v>783000</v>
       </c>
       <c r="I688" s="1" t="s">
-        <v>965</v>
+        <v>924</v>
       </c>
     </row>
     <row r="689" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H689" s="1">
-        <v>786001</v>
+        <v>783001</v>
       </c>
       <c r="I689" s="1" t="s">
-        <v>966</v>
+        <v>925</v>
       </c>
     </row>
     <row r="690" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H690" s="1">
-        <v>786002</v>
+        <v>783002</v>
       </c>
       <c r="I690" s="1" t="s">
-        <v>967</v>
+        <v>926</v>
       </c>
     </row>
     <row r="691" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H691" s="1">
-        <v>786099</v>
+        <v>783003</v>
       </c>
       <c r="I691" s="1" t="s">
-        <v>472</v>
+        <v>927</v>
       </c>
     </row>
     <row r="692" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D692" s="8">
-        <v>787</v>
-      </c>
-      <c r="E692" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F692" s="8"/>
-      <c r="G692" s="8"/>
-      <c r="H692" s="8"/>
-      <c r="I692" s="8"/>
+      <c r="H692" s="1">
+        <v>783004</v>
+      </c>
+      <c r="I692" s="1" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="693" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F693" s="9">
-        <v>7870</v>
-      </c>
-      <c r="G693" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="H693" s="9"/>
-      <c r="I693" s="9"/>
+      <c r="H693" s="1">
+        <v>783005</v>
+      </c>
+      <c r="I693" s="1" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="694" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H694" s="1">
-        <v>787000</v>
+        <v>783006</v>
       </c>
       <c r="I694" s="1" t="s">
-        <v>968</v>
+        <v>929</v>
       </c>
     </row>
     <row r="695" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H695" s="1">
-        <v>787001</v>
+        <v>783007</v>
       </c>
       <c r="I695" s="1" t="s">
-        <v>969</v>
+        <v>930</v>
       </c>
     </row>
     <row r="696" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H696" s="1">
-        <v>787002</v>
-      </c>
-      <c r="I696" s="1" t="s">
-        <v>970</v>
-      </c>
+      <c r="D696" s="8">
+        <v>784</v>
+      </c>
+      <c r="E696" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="F696" s="8"/>
+      <c r="G696" s="8"/>
+      <c r="H696" s="8"/>
+      <c r="I696" s="8"/>
     </row>
     <row r="697" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H697" s="1">
-        <v>787003</v>
-      </c>
-      <c r="I697" s="1" t="s">
-        <v>971</v>
-      </c>
+      <c r="F697" s="9">
+        <v>7840</v>
+      </c>
+      <c r="G697" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="H697" s="9"/>
+      <c r="I697" s="9"/>
     </row>
     <row r="698" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D698" s="8">
-        <v>788</v>
-      </c>
-      <c r="E698" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="F698" s="8"/>
-      <c r="G698" s="8"/>
-      <c r="H698" s="8"/>
-      <c r="I698" s="8"/>
+      <c r="H698" s="1">
+        <v>784000</v>
+      </c>
+      <c r="I698" s="1" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="699" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F699" s="9">
-        <v>7880</v>
-      </c>
-      <c r="G699" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="H699" s="9"/>
-      <c r="I699" s="9"/>
+      <c r="H699" s="1">
+        <v>784001</v>
+      </c>
+      <c r="I699" s="1" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="700" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H700" s="1">
-        <v>788000</v>
-      </c>
-      <c r="I700" s="1" t="s">
-        <v>972</v>
-      </c>
+      <c r="F700" s="9">
+        <v>7841</v>
+      </c>
+      <c r="G700" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="H700" s="9"/>
+      <c r="I700" s="9"/>
     </row>
     <row r="701" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H701" s="1">
-        <v>788001</v>
+        <v>784100</v>
       </c>
       <c r="I701" s="1" t="s">
-        <v>973</v>
+        <v>467</v>
       </c>
     </row>
     <row r="702" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H702" s="1">
-        <v>788002</v>
+        <v>784101</v>
       </c>
       <c r="I702" s="1" t="s">
-        <v>974</v>
+        <v>932</v>
       </c>
     </row>
     <row r="703" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H703" s="1">
-        <v>788003</v>
-      </c>
-      <c r="I703" s="1" t="s">
-        <v>975</v>
-      </c>
+      <c r="F703" s="9">
+        <v>7842</v>
+      </c>
+      <c r="G703" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="H703" s="9"/>
+      <c r="I703" s="9"/>
     </row>
     <row r="704" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H704" s="1">
-        <v>788004</v>
+        <v>784200</v>
       </c>
       <c r="I704" s="1" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="705" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B705" s="4">
-        <v>79</v>
-      </c>
-      <c r="C705" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="D705" s="4"/>
-      <c r="E705" s="4"/>
-      <c r="F705" s="4"/>
-      <c r="G705" s="4"/>
-      <c r="H705" s="4"/>
-      <c r="I705" s="4"/>
-    </row>
-    <row r="706" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D706" s="8">
-        <v>790</v>
-      </c>
-      <c r="E706" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F706" s="8"/>
-      <c r="G706" s="8"/>
-      <c r="H706" s="8"/>
-      <c r="I706" s="8"/>
-    </row>
-    <row r="707" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D707" s="8">
-        <v>797</v>
-      </c>
-      <c r="E707" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="F707" s="8"/>
-      <c r="G707" s="8"/>
-      <c r="H707" s="8"/>
-      <c r="I707" s="8"/>
-    </row>
-    <row r="708" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D708" s="8">
-        <v>799</v>
-      </c>
-      <c r="E708" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="F708" s="8"/>
-      <c r="G708" s="8"/>
-      <c r="H708" s="8"/>
-      <c r="I708" s="8"/>
-    </row>
-    <row r="709" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B709" s="4">
-        <v>50</v>
-      </c>
-      <c r="C709" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D709" s="4"/>
-      <c r="E709" s="4"/>
-      <c r="F709" s="4"/>
-      <c r="G709" s="4"/>
-      <c r="H709" s="4"/>
-      <c r="I709" s="4"/>
-    </row>
-    <row r="710" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D710" s="8">
-        <v>500</v>
-      </c>
-      <c r="E710" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="F710" s="8"/>
-      <c r="G710" s="8"/>
-      <c r="H710" s="8"/>
-      <c r="I710" s="8"/>
-    </row>
-    <row r="711" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F711" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G711" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="H711" s="9"/>
-      <c r="I711" s="9"/>
-    </row>
-    <row r="712" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H712" s="1">
-        <v>500000</v>
-      </c>
-      <c r="I712" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="713" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F713" s="9">
-        <v>5001</v>
-      </c>
-      <c r="G713" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="H713" s="9"/>
-      <c r="I713" s="9"/>
-    </row>
-    <row r="714" spans="2:9" x14ac:dyDescent="0.25">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="705" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H705" s="1">
+        <v>784201</v>
+      </c>
+      <c r="I705" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="706" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H706" s="1">
+        <v>784202</v>
+      </c>
+      <c r="I706" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="707" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H707" s="1">
+        <v>784203</v>
+      </c>
+      <c r="I707" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="708" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H708" s="1">
+        <v>784204</v>
+      </c>
+      <c r="I708" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="709" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H709" s="1">
+        <v>784205</v>
+      </c>
+      <c r="I709" s="1" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="710" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H710" s="1">
+        <v>784206</v>
+      </c>
+      <c r="I710" s="1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="711" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H711" s="1">
+        <v>784207</v>
+      </c>
+      <c r="I711" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="712" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F712" s="9">
+        <v>7843</v>
+      </c>
+      <c r="G712" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="H712" s="9"/>
+      <c r="I712" s="9"/>
+    </row>
+    <row r="713" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H713" s="1">
+        <v>784300</v>
+      </c>
+      <c r="I713" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="714" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H714" s="1">
-        <v>500100</v>
+        <v>784301</v>
       </c>
       <c r="I714" s="1" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="715" spans="2:9" x14ac:dyDescent="0.25">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="715" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H715" s="1">
-        <v>500101</v>
+        <v>784302</v>
       </c>
       <c r="I715" s="1" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="716" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F716" s="9">
-        <v>5002</v>
-      </c>
-      <c r="G716" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="H716" s="9"/>
-      <c r="I716" s="9"/>
-    </row>
-    <row r="717" spans="2:9" x14ac:dyDescent="0.25">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="716" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H716" s="1">
+        <v>784303</v>
+      </c>
+      <c r="I716" s="1" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="717" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H717" s="1">
-        <v>500200</v>
+        <v>784304</v>
       </c>
       <c r="I717" s="1" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="718" spans="2:9" x14ac:dyDescent="0.25">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="718" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H718" s="1">
-        <v>500201</v>
+        <v>784305</v>
       </c>
       <c r="I718" s="1" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="719" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F719" s="9">
-        <v>5003</v>
-      </c>
-      <c r="G719" s="9" t="s">
-        <v>476</v>
-      </c>
-      <c r="H719" s="9"/>
-      <c r="I719" s="9"/>
-    </row>
-    <row r="720" spans="2:9" x14ac:dyDescent="0.25">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="719" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H719" s="1">
+        <v>784306</v>
+      </c>
+      <c r="I719" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="720" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H720" s="1">
-        <v>500300</v>
+        <v>784307</v>
       </c>
       <c r="I720" s="1" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="721" spans="6:9" x14ac:dyDescent="0.25">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="721" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H721" s="1">
-        <v>500301</v>
+        <v>784308</v>
       </c>
       <c r="I721" s="1" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="722" spans="6:9" x14ac:dyDescent="0.25">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="722" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H722" s="1">
-        <v>500302</v>
+        <v>784309</v>
       </c>
       <c r="I722" s="1" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="723" spans="6:9" x14ac:dyDescent="0.25">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="723" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H723" s="1">
-        <v>500303</v>
+        <v>784310</v>
       </c>
       <c r="I723" s="1" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="724" spans="6:9" x14ac:dyDescent="0.25">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="724" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H724" s="1">
-        <v>500304</v>
+        <v>784311</v>
       </c>
       <c r="I724" s="1" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="725" spans="6:9" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="725" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H725" s="1">
-        <v>500305</v>
+        <v>784312</v>
       </c>
       <c r="I725" s="1" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="726" spans="6:9" x14ac:dyDescent="0.25">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="726" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H726" s="1">
-        <v>500306</v>
+        <v>784313</v>
       </c>
       <c r="I726" s="1" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="727" spans="6:9" x14ac:dyDescent="0.25">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="727" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H727" s="1">
-        <v>500307</v>
+        <v>784314</v>
       </c>
       <c r="I727" s="1" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="728" spans="6:9" x14ac:dyDescent="0.25">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="728" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H728" s="1">
-        <v>500308</v>
+        <v>784315</v>
       </c>
       <c r="I728" s="1" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="729" spans="6:9" x14ac:dyDescent="0.25">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="729" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H729" s="1">
-        <v>500309</v>
+        <v>784316</v>
       </c>
       <c r="I729" s="1" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="730" spans="6:9" x14ac:dyDescent="0.25">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="730" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H730" s="1">
-        <v>500310</v>
+        <v>784317</v>
       </c>
       <c r="I730" s="1" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="731" spans="6:9" x14ac:dyDescent="0.25">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="731" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H731" s="1">
-        <v>500311</v>
+        <v>784318</v>
       </c>
       <c r="I731" s="1" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="732" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F732" s="9">
-        <v>5004</v>
-      </c>
-      <c r="G732" s="9" t="s">
-        <v>477</v>
-      </c>
-      <c r="H732" s="9"/>
-      <c r="I732" s="9"/>
-    </row>
-    <row r="733" spans="6:9" x14ac:dyDescent="0.25">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="732" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H732" s="1">
+        <v>784319</v>
+      </c>
+      <c r="I732" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="733" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H733" s="1">
-        <v>500400</v>
+        <v>784320</v>
       </c>
       <c r="I733" s="1" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="734" spans="6:9" x14ac:dyDescent="0.25">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="734" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H734" s="1">
-        <v>500401</v>
+        <v>784321</v>
       </c>
       <c r="I734" s="1" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="735" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H735" s="1">
-        <v>500402</v>
-      </c>
-      <c r="I735" s="1" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="736" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H736" s="1">
-        <v>500403</v>
-      </c>
-      <c r="I736" s="1" t="s">
-        <v>996</v>
-      </c>
+        <v>962</v>
+      </c>
+    </row>
+    <row r="735" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D735" s="8">
+        <v>785</v>
+      </c>
+      <c r="E735" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="F735" s="8"/>
+      <c r="G735" s="8"/>
+      <c r="H735" s="8"/>
+      <c r="I735" s="8"/>
+    </row>
+    <row r="736" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F736" s="9">
+        <v>7850</v>
+      </c>
+      <c r="G736" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="H736" s="9"/>
+      <c r="I736" s="9"/>
     </row>
     <row r="737" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H737" s="1">
-        <v>500404</v>
+        <v>785000</v>
       </c>
       <c r="I737" s="1" t="s">
-        <v>997</v>
+        <v>470</v>
       </c>
     </row>
     <row r="738" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H738" s="1">
-        <v>500409</v>
+        <v>785001</v>
       </c>
       <c r="I738" s="1" t="s">
-        <v>998</v>
+        <v>963</v>
       </c>
     </row>
     <row r="739" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H739" s="1">
-        <v>500410</v>
-      </c>
-      <c r="I739" s="1" t="s">
-        <v>999</v>
-      </c>
+      <c r="F739" s="9">
+        <v>7851</v>
+      </c>
+      <c r="G739" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H739" s="9"/>
+      <c r="I739" s="9"/>
     </row>
     <row r="740" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H740" s="1">
-        <v>500411</v>
+        <v>785100</v>
       </c>
       <c r="I740" s="1" t="s">
-        <v>1000</v>
+        <v>471</v>
       </c>
     </row>
     <row r="741" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D741" s="8">
-        <v>501</v>
-      </c>
-      <c r="E741" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="F741" s="8"/>
-      <c r="G741" s="8"/>
-      <c r="H741" s="8"/>
-      <c r="I741" s="8"/>
+      <c r="H741" s="1">
+        <v>785101</v>
+      </c>
+      <c r="I741" s="1" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="742" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F742" s="9">
-        <v>5010</v>
-      </c>
-      <c r="G742" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="H742" s="9"/>
-      <c r="I742" s="9"/>
+      <c r="D742" s="8">
+        <v>786</v>
+      </c>
+      <c r="E742" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="F742" s="8"/>
+      <c r="G742" s="8"/>
+      <c r="H742" s="8"/>
+      <c r="I742" s="8"/>
     </row>
     <row r="743" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H743" s="1">
-        <v>501000</v>
-      </c>
-      <c r="I743" s="1" t="s">
-        <v>1001</v>
-      </c>
+      <c r="F743" s="9">
+        <v>7860</v>
+      </c>
+      <c r="G743" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="H743" s="9"/>
+      <c r="I743" s="9"/>
     </row>
     <row r="744" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H744" s="1">
-        <v>501001</v>
+        <v>786000</v>
       </c>
       <c r="I744" s="1" t="s">
-        <v>1002</v>
+        <v>965</v>
       </c>
     </row>
     <row r="745" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F745" s="9">
-        <v>5011</v>
-      </c>
-      <c r="G745" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="H745" s="9"/>
-      <c r="I745" s="9"/>
+      <c r="H745" s="1">
+        <v>786001</v>
+      </c>
+      <c r="I745" s="1" t="s">
+        <v>966</v>
+      </c>
     </row>
     <row r="746" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H746" s="1">
-        <v>501100</v>
+        <v>786002</v>
       </c>
       <c r="I746" s="1" t="s">
-        <v>1003</v>
+        <v>967</v>
       </c>
     </row>
     <row r="747" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H747" s="1">
-        <v>501101</v>
+        <v>786099</v>
       </c>
       <c r="I747" s="1" t="s">
-        <v>1004</v>
+        <v>472</v>
       </c>
     </row>
     <row r="748" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F748" s="9">
-        <v>5012</v>
-      </c>
-      <c r="G748" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="H748" s="9"/>
-      <c r="I748" s="9"/>
+      <c r="D748" s="8">
+        <v>787</v>
+      </c>
+      <c r="E748" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F748" s="8"/>
+      <c r="G748" s="8"/>
+      <c r="H748" s="8"/>
+      <c r="I748" s="8"/>
     </row>
     <row r="749" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H749" s="1">
-        <v>501200</v>
-      </c>
-      <c r="I749" s="1" t="s">
-        <v>1005</v>
-      </c>
+      <c r="F749" s="9">
+        <v>7870</v>
+      </c>
+      <c r="G749" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="H749" s="9"/>
+      <c r="I749" s="9"/>
     </row>
     <row r="750" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H750" s="1">
-        <v>501201</v>
+        <v>787000</v>
       </c>
       <c r="I750" s="1" t="s">
-        <v>1006</v>
+        <v>968</v>
       </c>
     </row>
     <row r="751" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F751" s="9">
-        <v>5013</v>
-      </c>
-      <c r="G751" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="H751" s="9"/>
-      <c r="I751" s="9"/>
+      <c r="H751" s="1">
+        <v>787001</v>
+      </c>
+      <c r="I751" s="1" t="s">
+        <v>969</v>
+      </c>
     </row>
     <row r="752" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H752" s="1">
+        <v>787002</v>
+      </c>
+      <c r="I752" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="753" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H753" s="1">
+        <v>787003</v>
+      </c>
+      <c r="I753" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="754" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D754" s="8">
+        <v>788</v>
+      </c>
+      <c r="E754" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="F754" s="8"/>
+      <c r="G754" s="8"/>
+      <c r="H754" s="8"/>
+      <c r="I754" s="8"/>
+    </row>
+    <row r="755" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F755" s="9">
+        <v>7880</v>
+      </c>
+      <c r="G755" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="H755" s="9"/>
+      <c r="I755" s="9"/>
+    </row>
+    <row r="756" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H756" s="1">
+        <v>788000</v>
+      </c>
+      <c r="I756" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="757" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H757" s="1">
+        <v>788001</v>
+      </c>
+      <c r="I757" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="758" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H758" s="1">
+        <v>788002</v>
+      </c>
+      <c r="I758" s="1" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="759" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H759" s="1">
+        <v>788003</v>
+      </c>
+      <c r="I759" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="760" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H760" s="1">
+        <v>788004</v>
+      </c>
+      <c r="I760" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="761" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B761" s="4">
+        <v>79</v>
+      </c>
+      <c r="C761" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D761" s="4"/>
+      <c r="E761" s="4"/>
+      <c r="F761" s="4"/>
+      <c r="G761" s="4"/>
+      <c r="H761" s="4"/>
+      <c r="I761" s="4"/>
+    </row>
+    <row r="762" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D762" s="8">
+        <v>790</v>
+      </c>
+      <c r="E762" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F762" s="8"/>
+      <c r="G762" s="8"/>
+      <c r="H762" s="8"/>
+      <c r="I762" s="8"/>
+    </row>
+    <row r="763" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D763" s="8">
+        <v>797</v>
+      </c>
+      <c r="E763" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F763" s="8"/>
+      <c r="G763" s="8"/>
+      <c r="H763" s="8"/>
+      <c r="I763" s="8"/>
+    </row>
+    <row r="764" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D764" s="8">
+        <v>799</v>
+      </c>
+      <c r="E764" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="F764" s="8"/>
+      <c r="G764" s="8"/>
+      <c r="H764" s="8"/>
+      <c r="I764" s="8"/>
+    </row>
+    <row r="765" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B765" s="4">
+        <v>50</v>
+      </c>
+      <c r="C765" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D765" s="4"/>
+      <c r="E765" s="4"/>
+      <c r="F765" s="4"/>
+      <c r="G765" s="4"/>
+      <c r="H765" s="4"/>
+      <c r="I765" s="4"/>
+    </row>
+    <row r="766" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D766" s="8">
+        <v>500</v>
+      </c>
+      <c r="E766" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="F766" s="8"/>
+      <c r="G766" s="8"/>
+      <c r="H766" s="8"/>
+      <c r="I766" s="8"/>
+    </row>
+    <row r="767" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F767" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G767" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="H767" s="9"/>
+      <c r="I767" s="9"/>
+    </row>
+    <row r="768" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H768" s="1">
+        <v>500000</v>
+      </c>
+      <c r="I768" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="769" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F769" s="9">
+        <v>5001</v>
+      </c>
+      <c r="G769" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="H769" s="9"/>
+      <c r="I769" s="9"/>
+    </row>
+    <row r="770" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H770" s="1">
+        <v>500100</v>
+      </c>
+      <c r="I770" s="1" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="771" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H771" s="1">
+        <v>500101</v>
+      </c>
+      <c r="I771" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="772" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F772" s="9">
+        <v>5002</v>
+      </c>
+      <c r="G772" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="H772" s="9"/>
+      <c r="I772" s="9"/>
+    </row>
+    <row r="773" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H773" s="1">
+        <v>500200</v>
+      </c>
+      <c r="I773" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="774" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H774" s="1">
+        <v>500201</v>
+      </c>
+      <c r="I774" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="775" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F775" s="9">
+        <v>5003</v>
+      </c>
+      <c r="G775" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="H775" s="9"/>
+      <c r="I775" s="9"/>
+    </row>
+    <row r="776" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H776" s="1">
+        <v>500300</v>
+      </c>
+      <c r="I776" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="777" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H777" s="1">
+        <v>500301</v>
+      </c>
+      <c r="I777" s="1" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="778" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H778" s="1">
+        <v>500302</v>
+      </c>
+      <c r="I778" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="779" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H779" s="1">
+        <v>500303</v>
+      </c>
+      <c r="I779" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="780" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H780" s="1">
+        <v>500304</v>
+      </c>
+      <c r="I780" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="781" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H781" s="1">
+        <v>500305</v>
+      </c>
+      <c r="I781" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="782" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H782" s="1">
+        <v>500306</v>
+      </c>
+      <c r="I782" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="783" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H783" s="1">
+        <v>500307</v>
+      </c>
+      <c r="I783" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="784" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H784" s="1">
+        <v>500308</v>
+      </c>
+      <c r="I784" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="785" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H785" s="1">
+        <v>500309</v>
+      </c>
+      <c r="I785" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="786" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H786" s="1">
+        <v>500310</v>
+      </c>
+      <c r="I786" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="787" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H787" s="1">
+        <v>500311</v>
+      </c>
+      <c r="I787" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="788" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F788" s="9">
+        <v>5004</v>
+      </c>
+      <c r="G788" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="H788" s="9"/>
+      <c r="I788" s="9"/>
+    </row>
+    <row r="789" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H789" s="1">
+        <v>500400</v>
+      </c>
+      <c r="I789" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="790" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H790" s="1">
+        <v>500401</v>
+      </c>
+      <c r="I790" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="791" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H791" s="1">
+        <v>500402</v>
+      </c>
+      <c r="I791" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="792" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H792" s="1">
+        <v>500403</v>
+      </c>
+      <c r="I792" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="793" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H793" s="1">
+        <v>500404</v>
+      </c>
+      <c r="I793" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="794" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H794" s="1">
+        <v>500409</v>
+      </c>
+      <c r="I794" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="795" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H795" s="1">
+        <v>500410</v>
+      </c>
+      <c r="I795" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="796" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H796" s="1">
+        <v>500411</v>
+      </c>
+      <c r="I796" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="797" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D797" s="8">
+        <v>501</v>
+      </c>
+      <c r="E797" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="F797" s="8"/>
+      <c r="G797" s="8"/>
+      <c r="H797" s="8"/>
+      <c r="I797" s="8"/>
+    </row>
+    <row r="798" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F798" s="9">
+        <v>5010</v>
+      </c>
+      <c r="G798" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="H798" s="9"/>
+      <c r="I798" s="9"/>
+    </row>
+    <row r="799" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H799" s="1">
+        <v>501000</v>
+      </c>
+      <c r="I799" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="800" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H800" s="1">
+        <v>501001</v>
+      </c>
+      <c r="I800" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="801" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F801" s="9">
+        <v>5011</v>
+      </c>
+      <c r="G801" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="H801" s="9"/>
+      <c r="I801" s="9"/>
+    </row>
+    <row r="802" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H802" s="1">
+        <v>501100</v>
+      </c>
+      <c r="I802" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="803" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H803" s="1">
+        <v>501101</v>
+      </c>
+      <c r="I803" s="1" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="804" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F804" s="9">
+        <v>5012</v>
+      </c>
+      <c r="G804" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="H804" s="9"/>
+      <c r="I804" s="9"/>
+    </row>
+    <row r="805" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H805" s="1">
+        <v>501200</v>
+      </c>
+      <c r="I805" s="1" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="806" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H806" s="1">
+        <v>501201</v>
+      </c>
+      <c r="I806" s="1" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="807" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F807" s="9">
+        <v>5013</v>
+      </c>
+      <c r="G807" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="H807" s="9"/>
+      <c r="I807" s="9"/>
+    </row>
+    <row r="808" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H808" s="1">
         <v>501300</v>
       </c>
-      <c r="I752" s="1" t="s">
+      <c r="I808" s="1" t="s">
         <v>1007</v>
       </c>
     </row>
-    <row r="753" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H753" s="1">
+    <row r="809" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H809" s="1">
         <v>501301</v>
       </c>
-      <c r="I753" s="1" t="s">
+      <c r="I809" s="1" t="s">
         <v>1008</v>
       </c>
     </row>
-    <row r="754" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F754" s="9">
+    <row r="810" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F810" s="9">
         <v>5014</v>
       </c>
-      <c r="G754" s="9" t="s">
+      <c r="G810" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="H754" s="9"/>
-      <c r="I754" s="9"/>
-    </row>
-    <row r="755" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H755" s="1">
+      <c r="H810" s="9"/>
+      <c r="I810" s="9"/>
+    </row>
+    <row r="811" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H811" s="1">
         <v>501400</v>
       </c>
-      <c r="I755" s="1" t="s">
+      <c r="I811" s="1" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="756" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H756" s="1">
+    <row r="812" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H812" s="1">
         <v>501401</v>
       </c>
-      <c r="I756" s="1" t="s">
+      <c r="I812" s="1" t="s">
         <v>1010</v>
       </c>
     </row>

</xml_diff>